<commit_message>
update tables with SST and other stuff
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmz5202/Software/tgw-tc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40972A48-C80E-8642-A747-1DD396DA94ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8A9364-7A96-3F4F-8AA6-852771AA70EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15560" windowHeight="21580" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="statistics_output" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="144">
   <si>
     <t>Variable</t>
   </si>
@@ -465,6 +465,12 @@
   </si>
   <si>
     <t>Definition</t>
+  </si>
+  <si>
+    <t>dSST(K)</t>
+  </si>
+  <si>
+    <t>SST</t>
   </si>
 </sst>
 </file>
@@ -959,7 +965,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -976,6 +982,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3671,7 +3678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402EA909-F4C2-A34F-864D-41FFD39D614E}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
@@ -3766,7 +3773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BS9"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" workbookViewId="0">
+    <sheetView topLeftCell="AX1" workbookViewId="0">
       <selection activeCell="AK3" sqref="AK3:AO3"/>
     </sheetView>
   </sheetViews>
@@ -5970,10 +5977,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CC06A6-9503-D742-8415-062A32654C15}">
-  <dimension ref="A1:Z25"/>
+  <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z10" sqref="K1:Z10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6503,101 +6510,628 @@
         <v>6.6963794140570521E-2</v>
       </c>
     </row>
-    <row r="21" spans="12:20" x14ac:dyDescent="0.2">
-      <c r="Q21" t="s">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="D12" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" s="5"/>
+      <c r="L12" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="O12" t="s">
+        <v>82</v>
+      </c>
+      <c r="P12" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>93</v>
+      </c>
+      <c r="R12" t="s">
+        <v>94</v>
+      </c>
+      <c r="S12" t="s">
+        <v>96</v>
+      </c>
+      <c r="T12" t="s">
+        <v>97</v>
+      </c>
+      <c r="U12" t="s">
+        <v>91</v>
+      </c>
+      <c r="V12" t="s">
+        <v>92</v>
+      </c>
+      <c r="W12" t="s">
+        <v>98</v>
+      </c>
+      <c r="X12" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13">
+        <v>0.7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K13" t="s">
+        <v>105</v>
+      </c>
+      <c r="M13" s="10">
+        <v>299.54677172874801</v>
+      </c>
+      <c r="O13">
+        <v>22.3</v>
+      </c>
+      <c r="P13">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="U13">
+        <v>52.6</v>
+      </c>
+      <c r="V13">
+        <v>80.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>4.5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15">
+        <v>3.1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>4.5</v>
+      </c>
+      <c r="G15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16">
+        <v>4.5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>4.5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17">
+        <v>6.7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>4.5</v>
+      </c>
+      <c r="G17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>8.5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" t="s">
+        <v>62</v>
+      </c>
+      <c r="K18" t="s">
+        <v>101</v>
+      </c>
+      <c r="M18" s="10">
+        <v>300.71680754536698</v>
+      </c>
+      <c r="N18" s="6">
+        <f>M18-M$13</f>
+        <v>1.1700358166189631</v>
+      </c>
+      <c r="O18">
+        <v>26</v>
+      </c>
+      <c r="P18">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="Q18" s="7">
+        <f>(O18-O$2)/O$2</f>
+        <v>0.16591928251121071</v>
+      </c>
+      <c r="R18" s="7">
+        <f>(P18-P$2)/P$2</f>
+        <v>0.1023391812865497</v>
+      </c>
+      <c r="S18" s="7">
+        <f>Q18/$N18</f>
+        <v>0.14180701150727629</v>
+      </c>
+      <c r="T18" s="7">
+        <f>R18/$N18</f>
+        <v>8.7466708140848087E-2</v>
+      </c>
+      <c r="U18">
+        <v>58.9</v>
+      </c>
+      <c r="V18">
+        <v>89.1</v>
+      </c>
+      <c r="W18" s="7">
+        <f>(U18-U$2)/U$2</f>
+        <v>0.11977186311787066</v>
+      </c>
+      <c r="X18" s="7">
+        <f>(V18-V$2)/V$2</f>
+        <v>0.10272277227722769</v>
+      </c>
+      <c r="Y18" s="7">
+        <f>W18/$N18</f>
+        <v>0.10236598009792026</v>
+      </c>
+      <c r="Z18" s="7">
+        <f>X18/$N18</f>
+        <v>8.7794553652267085E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>8.5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" t="s">
+        <v>59</v>
+      </c>
+      <c r="K19" t="s">
+        <v>102</v>
+      </c>
+      <c r="M19" s="10">
+        <v>301.20086914995198</v>
+      </c>
+      <c r="N19" s="6">
+        <f t="shared" ref="N19:N21" si="8">M19-M$13</f>
+        <v>1.6540974212039714</v>
+      </c>
+      <c r="O19">
+        <v>27.5</v>
+      </c>
+      <c r="P19">
+        <v>78</v>
+      </c>
+      <c r="Q19" s="7">
+        <f t="shared" ref="Q19:Q21" si="9">(O19-O$2)/O$2</f>
+        <v>0.2331838565022421</v>
+      </c>
+      <c r="R19" s="7">
+        <f t="shared" ref="R19:R21" si="10">(P19-P$2)/P$2</f>
+        <v>0.14035087719298237</v>
+      </c>
+      <c r="S19" s="7">
+        <f t="shared" ref="S19:S21" si="11">Q19/$N19</f>
+        <v>0.14097347200536356</v>
+      </c>
+      <c r="T19" s="7">
+        <f>R19/N19</f>
+        <v>8.4850429843983957E-2</v>
+      </c>
+      <c r="U19">
+        <v>62.6</v>
+      </c>
+      <c r="V19">
+        <v>92.5</v>
+      </c>
+      <c r="W19" s="7">
+        <f t="shared" ref="W19:W21" si="12">(U19-U$2)/U$2</f>
+        <v>0.19011406844106463</v>
+      </c>
+      <c r="X19" s="7">
+        <f t="shared" ref="X19:X21" si="13">(V19-V$2)/V$2</f>
+        <v>0.14480198019801985</v>
+      </c>
+      <c r="Y19" s="7">
+        <f t="shared" ref="Y19:Y21" si="14">W19/$N19</f>
+        <v>0.11493523053961713</v>
+      </c>
+      <c r="Z19" s="7">
+        <f t="shared" ref="Z19:Z21" si="15">X19/$N19</f>
+        <v>8.7541385617192075E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>8.5</v>
+      </c>
+      <c r="G20" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K20" t="s">
+        <v>103</v>
+      </c>
+      <c r="M20" s="10">
+        <v>302.15503581661801</v>
+      </c>
+      <c r="N20" s="6">
+        <f t="shared" si="8"/>
+        <v>2.6082640878699976</v>
+      </c>
+      <c r="O20">
+        <v>30.1</v>
+      </c>
+      <c r="P20">
+        <v>84.8</v>
+      </c>
+      <c r="Q20" s="7">
+        <f t="shared" si="9"/>
+        <v>0.34977578475336324</v>
+      </c>
+      <c r="R20" s="7">
+        <f t="shared" si="10"/>
+        <v>0.23976608187134488</v>
+      </c>
+      <c r="S20" s="7">
+        <f t="shared" si="11"/>
+        <v>0.13410290253200655</v>
+      </c>
+      <c r="T20" s="7">
+        <f>R20/N20</f>
+        <v>9.1925538900145071E-2</v>
+      </c>
+      <c r="U20">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="V20">
+        <v>100.2</v>
+      </c>
+      <c r="W20" s="7">
+        <f t="shared" si="12"/>
+        <v>0.27566539923954358</v>
+      </c>
+      <c r="X20" s="7">
+        <f t="shared" si="13"/>
+        <v>0.24009900990099017</v>
+      </c>
+      <c r="Y20" s="7">
+        <f t="shared" si="14"/>
+        <v>0.10568922085825361</v>
+      </c>
+      <c r="Z20" s="7">
+        <f t="shared" si="15"/>
+        <v>9.2053182427958694E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>8.5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" t="s">
+        <v>53</v>
+      </c>
+      <c r="I21" t="s">
+        <v>52</v>
+      </c>
+      <c r="K21" t="s">
+        <v>104</v>
+      </c>
+      <c r="M21" s="10">
+        <v>303.35076886341898</v>
+      </c>
+      <c r="N21" s="6">
+        <f t="shared" si="8"/>
+        <v>3.8039971346709649</v>
+      </c>
+      <c r="O21">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="P21">
+        <v>93</v>
+      </c>
+      <c r="Q21" s="7">
+        <f t="shared" si="9"/>
+        <v>0.5112107623318386</v>
+      </c>
+      <c r="R21" s="7">
+        <f t="shared" si="10"/>
+        <v>0.35964912280701744</v>
+      </c>
+      <c r="S21" s="7">
+        <f t="shared" si="11"/>
+        <v>0.13438778848503441</v>
+      </c>
+      <c r="T21" s="7">
+        <f>R21/N21</f>
+        <v>9.4545056180260795E-2</v>
+      </c>
+      <c r="U21">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="V21">
+        <v>111.4</v>
+      </c>
+      <c r="W21" s="7">
+        <f t="shared" si="12"/>
+        <v>0.44676806083650178</v>
+      </c>
+      <c r="X21" s="7">
+        <f t="shared" si="13"/>
+        <v>0.37871287128712883</v>
+      </c>
+      <c r="Y21" s="7">
+        <f t="shared" si="14"/>
+        <v>0.11744700246078024</v>
+      </c>
+      <c r="Z21" s="7">
+        <f t="shared" si="15"/>
+        <v>9.9556560607106354E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Q30" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="12:20" x14ac:dyDescent="0.2">
-      <c r="L22">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="H31" s="10">
+        <v>299.54677172874801</v>
+      </c>
+      <c r="L31">
         <v>2.2999999999999998</v>
       </c>
-      <c r="N22">
-        <f>L22-$L$2</f>
+      <c r="N31">
+        <f>L31-$L$2</f>
         <v>1.5999999999999999</v>
       </c>
-      <c r="Q22">
+      <c r="Q31">
         <v>13.5</v>
       </c>
-      <c r="R22">
+      <c r="R31">
         <v>10.199999999999999</v>
       </c>
-      <c r="S22">
-        <f>Q22/N22</f>
+      <c r="S31">
+        <f>Q31/N31</f>
         <v>8.4375</v>
       </c>
-      <c r="T22">
-        <f>R22/N22</f>
+      <c r="T31">
+        <f>R31/N31</f>
         <v>6.375</v>
       </c>
     </row>
-    <row r="23" spans="12:20" x14ac:dyDescent="0.2">
-      <c r="L23">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="H32" s="10">
+        <v>300.71680754536698</v>
+      </c>
+      <c r="L32">
         <v>3.1</v>
       </c>
-      <c r="N23">
-        <f>L23-$L$2</f>
+      <c r="N32">
+        <f>L32-$L$2</f>
         <v>2.4000000000000004</v>
       </c>
-      <c r="Q23">
+      <c r="Q32">
         <v>20.100000000000001</v>
       </c>
-      <c r="R23">
+      <c r="R32">
         <v>14</v>
       </c>
-      <c r="S23">
-        <f>Q23/N23</f>
+      <c r="S32">
+        <f>Q32/N32</f>
         <v>8.375</v>
       </c>
-      <c r="T23">
-        <f>R23/N23</f>
+      <c r="T32">
+        <f>R32/N32</f>
         <v>5.8333333333333321</v>
       </c>
     </row>
-    <row r="24" spans="12:20" x14ac:dyDescent="0.2">
-      <c r="L24">
+    <row r="33" spans="8:20" x14ac:dyDescent="0.2">
+      <c r="H33" s="10">
+        <v>301.20086914995198</v>
+      </c>
+      <c r="L33">
         <v>4.5</v>
       </c>
-      <c r="N24">
-        <f>L24-$L$2</f>
+      <c r="N33">
+        <f>L33-$L$2</f>
         <v>3.8</v>
       </c>
-      <c r="Q24">
+      <c r="Q33">
         <v>31.4</v>
       </c>
-      <c r="R24">
+      <c r="R33">
         <v>24</v>
       </c>
-      <c r="S24">
-        <f>Q24/N24</f>
+      <c r="S33">
+        <f>Q33/N33</f>
         <v>8.2631578947368425</v>
       </c>
-      <c r="T24">
-        <f>R24/N24</f>
+      <c r="T33">
+        <f>R33/N33</f>
         <v>6.3157894736842106</v>
       </c>
     </row>
-    <row r="25" spans="12:20" x14ac:dyDescent="0.2">
-      <c r="L25">
+    <row r="34" spans="8:20" x14ac:dyDescent="0.2">
+      <c r="H34" s="10">
+        <v>302.15503581661801</v>
+      </c>
+      <c r="L34">
         <v>6.7</v>
       </c>
-      <c r="N25">
-        <f>L25-$L$2</f>
+      <c r="N34">
+        <f>L34-$L$2</f>
         <v>6</v>
       </c>
-      <c r="Q25">
+      <c r="Q34">
         <v>47.2</v>
       </c>
-      <c r="R25">
+      <c r="R34">
         <v>36</v>
       </c>
-      <c r="S25">
-        <f>Q25/N25</f>
+      <c r="S34">
+        <f>Q34/N34</f>
         <v>7.8666666666666671</v>
       </c>
-      <c r="T25">
-        <f>R25/N25</f>
+      <c r="T34">
+        <f>R34/N34</f>
         <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="8:20" x14ac:dyDescent="0.2">
+      <c r="H35" s="10">
+        <v>303.35076886341898</v>
       </c>
     </row>
   </sheetData>
@@ -6607,10 +7141,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56DF0ABC-2771-8447-8A8A-C73AB93619B6}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="G10" sqref="G10:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6808,6 +7342,202 @@
         <v>7.8997273984266023E-2</v>
       </c>
       <c r="K6" s="7">
+        <v>6.6963794140570521E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" t="s">
+        <v>91</v>
+      </c>
+      <c r="I8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" t="s">
+        <v>110</v>
+      </c>
+      <c r="K8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="10">
+        <v>299.54677172874801</v>
+      </c>
+      <c r="D9" s="6">
+        <v>22.3</v>
+      </c>
+      <c r="E9" s="6">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="H9">
+        <v>52.6</v>
+      </c>
+      <c r="I9">
+        <v>80.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="10">
+        <v>300.71680754536698</v>
+      </c>
+      <c r="C10" s="6">
+        <f>B10-B9</f>
+        <v>1.1700358166189631</v>
+      </c>
+      <c r="D10" s="6">
+        <v>26</v>
+      </c>
+      <c r="E10" s="6">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0.14180701150727629</v>
+      </c>
+      <c r="G10" s="7">
+        <v>8.7466708140848087E-2</v>
+      </c>
+      <c r="H10">
+        <v>58.9</v>
+      </c>
+      <c r="I10">
+        <v>89.1</v>
+      </c>
+      <c r="J10" s="7">
+        <v>7.260404785123549E-2</v>
+      </c>
+      <c r="K10" s="7">
+        <v>6.226912464814631E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="10">
+        <v>301.20086914995198</v>
+      </c>
+      <c r="C11" s="6">
+        <f t="shared" ref="C11:C13" si="0">B11-B10</f>
+        <v>0.48406160458500835</v>
+      </c>
+      <c r="D11" s="6">
+        <v>27.5</v>
+      </c>
+      <c r="E11" s="6">
+        <v>78</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0.14097347200536356</v>
+      </c>
+      <c r="G11" s="7">
+        <v>8.4850429843983957E-2</v>
+      </c>
+      <c r="H11">
+        <v>62.6</v>
+      </c>
+      <c r="I11">
+        <v>92.5</v>
+      </c>
+      <c r="J11" s="7">
+        <v>8.0141738961263684E-2</v>
+      </c>
+      <c r="K11" s="7">
+        <v>6.1040629940025883E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="10">
+        <v>302.15503581661801</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" si="0"/>
+        <v>0.95416666666602623</v>
+      </c>
+      <c r="D12" s="6">
+        <v>30.1</v>
+      </c>
+      <c r="E12" s="6">
+        <v>84.8</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0.13410290253200655</v>
+      </c>
+      <c r="G12" s="7">
+        <v>9.1925538900145071E-2</v>
+      </c>
+      <c r="H12">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="I12">
+        <v>100.2</v>
+      </c>
+      <c r="J12" s="7">
+        <v>7.2405946072541222E-2</v>
+      </c>
+      <c r="K12" s="7">
+        <v>6.3064120527709142E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="10">
+        <v>303.35076886341898</v>
+      </c>
+      <c r="C13" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1957330468009673</v>
+      </c>
+      <c r="D13" s="6">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="E13" s="6">
+        <v>93</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0.13438778848503441</v>
+      </c>
+      <c r="G13" s="7">
+        <v>9.4545056180260795E-2</v>
+      </c>
+      <c r="H13">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="I13">
+        <v>111.4</v>
+      </c>
+      <c r="J13" s="7">
+        <v>7.8997273984266023E-2</v>
+      </c>
+      <c r="K13" s="7">
         <v>6.6963794140570521E-2</v>
       </c>
     </row>

</xml_diff>